<commit_message>
Adds paleointensity test_data result excel table
</commit_message>
<xml_diff>
--- a/RockPy/tests/test_data/SPD_Test_Data_Table.xlsx
+++ b/RockPy/tests/test_data/SPD_Test_Data_Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="10600"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30740" windowHeight="14860"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="6" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>VM1F</t>
   </si>
   <si>
-    <t>β</t>
-  </si>
-  <si>
     <t>Dec_Anc</t>
   </si>
   <si>
@@ -948,6 +945,9 @@
   </si>
   <si>
     <t>ET2_187A</t>
+  </si>
+  <si>
+    <t>beta</t>
   </si>
 </sst>
 </file>
@@ -1135,8 +1135,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1186,11 +1188,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1494,7 +1498,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="480" activePane="topRight"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1559,19 +1563,19 @@
   <sheetData>
     <row r="1" spans="1:62" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>0</v>
@@ -1580,25 +1584,25 @@
         <v>1</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="J1" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>4</v>
@@ -1613,22 +1617,22 @@
         <v>7</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="Y1" s="6" t="s">
         <v>9</v>
@@ -1640,46 +1644,46 @@
         <v>11</v>
       </c>
       <c r="AB1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AI1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="AJ1" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="AK1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="AL1" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AM1" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AN1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="AO1" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AP1" s="6" t="s">
         <v>14</v>
@@ -1697,57 +1701,57 @@
         <v>18</v>
       </c>
       <c r="AU1" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AV1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="AW1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AX1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AY1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AZ1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AZ1" s="6" t="s">
+      <c r="BA1" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="BA1" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="BB1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="BC1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD1" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="BD1" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="BE1" s="6" t="s">
         <v>21</v>
       </c>
       <c r="BF1" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BG1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="BH1" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BI1" s="6" t="s">
         <v>33</v>
       </c>
       <c r="BJ1" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3">
         <v>50</v>
@@ -1935,7 +1939,7 @@
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="3">
         <v>50</v>
@@ -3063,7 +3067,7 @@
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3">
         <v>60</v>
@@ -3627,7 +3631,7 @@
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="3">
         <v>30</v>
@@ -5131,7 +5135,7 @@
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="3">
         <v>50.3</v>
@@ -5535,30 +5539,30 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>89</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3">
         <v>44.1</v>
@@ -5585,7 +5589,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="3">
         <v>43.3</v>
@@ -5747,7 +5751,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3">
         <v>52.1</v>
@@ -5855,7 +5859,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="3">
         <v>55.6</v>
@@ -6146,7 +6150,7 @@
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="15">
         <v>66.3</v>
@@ -6158,7 +6162,7 @@
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="15">
         <f>F23/E23</f>
@@ -6167,7 +6171,7 @@
     </row>
     <row r="30" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1">
         <f>SQRT((C23*G23)/( (C23-1)*E23))</f>

</xml_diff>